<commit_message>
Affiche la carte google maps sur les page concerné
</commit_message>
<xml_diff>
--- a/Version 2/Documentation/plannification_detaillee.xlsx
+++ b/Version 2/Documentation/plannification_detaillee.xlsx
@@ -24,7 +24,7 @@
     <author>Antonio PISANELLO</author>
   </authors>
   <commentList>
-    <comment ref="B7" authorId="0">
+    <comment ref="B8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>Fonctionnalités</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Base de donnée</t>
+  </si>
+  <si>
+    <t>API Google maps</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +203,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +336,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -397,6 +406,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -743,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -840,23 +852,23 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="8">
-        <v>2</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="14"/>
+        <v>15</v>
+      </c>
+      <c r="B5" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="8">
         <v>2</v>
@@ -872,10 +884,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13" t="s">
@@ -888,41 +900,41 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="D8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" s="8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="16" t="s">
-        <v>10</v>
-      </c>
+      <c r="E9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="12"/>
       <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B10" s="8">
         <v>4</v>
@@ -930,36 +942,49 @@
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8">
+        <v>4</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -967,10 +992,13 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>